<commit_message>
south korea national inventory updates. change scaling mapping, fix some references, add user added data from the old korean inventory
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/Korea/Korea_CAPSS_Emissions.xlsx
+++ b/input/emissions-inventories/Korea/Korea_CAPSS_Emissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rach919/CEDS/CEDS/input/emissions-inventories/Korea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8919AF6D-0B47-6043-8DA2-361FEF46ABF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A38FD0-6830-2846-BC7A-43A022093814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="1940" windowWidth="23760" windowHeight="15580" firstSheet="7" activeTab="19" xr2:uid="{8B17AF1C-6E15-4850-AD0A-8FF427B3FCF7}"/>
+    <workbookView xWindow="14160" yWindow="500" windowWidth="23760" windowHeight="15580" firstSheet="10" activeTab="22" xr2:uid="{8B17AF1C-6E15-4850-AD0A-8FF427B3FCF7}"/>
   </bookViews>
   <sheets>
     <sheet name="1999" sheetId="21" r:id="rId1"/>
@@ -257,7 +257,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +267,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -336,13 +348,25 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -663,7 +687,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -681,21 +705,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1012,21 +1036,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1387,21 +1411,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1762,21 +1786,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2137,21 +2161,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2530,21 +2554,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2923,21 +2947,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3316,21 +3340,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3727,21 +3751,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4192,21 +4216,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -4657,21 +4681,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -5122,21 +5146,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -5434,7 +5458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8995C69-36F1-7544-8757-1CD7375662FC}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -5453,21 +5477,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -5918,23 +5942,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6384,23 +6408,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6832,8 +6856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C1E91AF-07E3-364E-8075-419ABF7F7FB2}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6851,23 +6875,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7033,14 +7057,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3">
+      <c r="G7" s="7">
         <v>24107</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -7056,67 +7080,67 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="9">
         <v>3498</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="9">
         <v>3218</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="9">
         <v>3498</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="9">
         <v>248</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="9">
         <v>287279</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="9">
         <v>29502</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="9">
         <v>1706</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="9">
         <v>134629</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="9">
         <v>1853</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="9">
         <v>16009</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="9">
         <v>14865</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="9">
         <v>16009</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="9">
         <v>8451</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="9">
         <v>281764</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="9">
         <v>64810</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="9">
         <v>111</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="9">
         <v>176633</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="9">
         <v>5990</v>
       </c>
     </row>
@@ -7317,21 +7341,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -7680,21 +7704,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -8043,21 +8067,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -8406,21 +8430,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -8769,21 +8793,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -9132,21 +9156,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -9495,21 +9519,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
adding EDGAR HTAP v3 korea scaling, fixing other scaling, clean up files
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/Korea/Korea_CAPSS_Emissions.xlsx
+++ b/input/emissions-inventories/Korea/Korea_CAPSS_Emissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rach919/CEDS/CEDS/input/emissions-inventories/Korea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A38FD0-6830-2846-BC7A-43A022093814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD97C36-2955-7049-8236-E0342E351E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="500" windowWidth="23760" windowHeight="15580" firstSheet="10" activeTab="22" xr2:uid="{8B17AF1C-6E15-4850-AD0A-8FF427B3FCF7}"/>
+    <workbookView xWindow="5040" yWindow="500" windowWidth="23760" windowHeight="15580" firstSheet="10" activeTab="22" xr2:uid="{8B17AF1C-6E15-4850-AD0A-8FF427B3FCF7}"/>
   </bookViews>
   <sheets>
     <sheet name="1999" sheetId="21" r:id="rId1"/>
@@ -335,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -351,12 +351,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -368,6 +362,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -706,17 +703,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1037,17 +1034,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1412,17 +1409,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1787,17 +1784,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -2162,17 +2159,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -2555,17 +2552,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -2948,17 +2945,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -3341,17 +3338,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -3752,17 +3749,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -4217,17 +4214,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -4682,17 +4679,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -5147,17 +5144,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -5478,17 +5475,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -5924,7 +5921,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5942,23 +5939,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6376,8 +6373,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6390,7 +6386,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6408,23 +6404,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6842,8 +6838,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -6857,7 +6852,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6875,23 +6870,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7057,7 +7052,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>24107</v>
       </c>
       <c r="H7" s="3"/>
@@ -7080,67 +7075,67 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+    <row r="9" spans="1:10" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>3498</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>3218</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>3498</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>248</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>287279</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>29502</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <v>1706</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>134629</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <v>1853</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:10" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>16009</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>14865</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="7">
         <v>16009</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>8451</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>281764</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="7">
         <v>64810</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="7">
         <v>111</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="7">
         <v>176633</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <v>5990</v>
       </c>
     </row>
@@ -7309,8 +7304,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:A2"/>
+  <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7342,17 +7336,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -7705,17 +7699,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -8068,17 +8062,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -8431,17 +8425,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -8794,17 +8788,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -9157,17 +9151,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -9520,17 +9514,17 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">

</xml_diff>